<commit_message>
added work to be done
</commit_message>
<xml_diff>
--- a/WeightedMeanCalculation.xlsx
+++ b/WeightedMeanCalculation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="180" documentId="8_{AA26790B-BFE9-4EA2-B98C-C9058616F0A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A8E7267-4D0A-4F75-BCF7-966742A492BB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD5B09F-D434-4E4B-B869-869ACAEA5E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="870" windowWidth="24495" windowHeight="11385" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>FROM:</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t>_nWeights2</t>
+  </si>
+  <si>
+    <t>How do I want to deal with the divide by 0?</t>
+  </si>
+  <si>
+    <t>Also, how to deal with the discontinuity in the battery curves?</t>
   </si>
 </sst>
 </file>
@@ -358,20 +364,18 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="14">
@@ -393,30 +397,6 @@
   <dxfs count="16">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor rgb="FFFDF5E9"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -537,6 +517,30 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor rgb="FFFDF5E9"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -670,7 +674,7 @@
     <tableColumn id="1" xr3:uid="{103AC109-718B-473E-B5BB-68C17DF04721}" name="Index"/>
     <tableColumn id="2" xr3:uid="{B90210B2-15C9-4D97-9BD4-7131548AFA35}" name="A"/>
     <tableColumn id="3" xr3:uid="{74FC5D26-9607-4547-A790-88ACB7444D05}" name="B"/>
-    <tableColumn id="4" xr3:uid="{A2BFE91E-BF9B-44A2-B163-2B8345AC55B3}" name="Mean" dataDxfId="7">
+    <tableColumn id="4" xr3:uid="{A2BFE91E-BF9B-44A2-B163-2B8345AC55B3}" name="Mean" dataDxfId="8">
       <calculatedColumnFormula array="1">_xlfn.LAMBDA(_xlpm.z, _xlfn.LET(_xlpm.x, ISNUMBER(_xlpm.z)*(_xlpm.z&lt;&gt;0),SUMPRODUCT(_xlpm.z,_nWeights,_xlpm.x)/SUMPRODUCT(_xlpm.x,_nWeights)))(Table1[[#This Row],[A]:[B]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -685,7 +689,7 @@
     <tableColumn id="1" xr3:uid="{E1B06609-4B61-41D4-9A7F-97B2F6509A51}" name="Index"/>
     <tableColumn id="2" xr3:uid="{5E0EFA48-44E4-4AB1-8629-E4E0EC01C105}" name="A"/>
     <tableColumn id="3" xr3:uid="{655E21ED-C630-43E6-B77D-915418726896}" name="B"/>
-    <tableColumn id="4" xr3:uid="{52D8179B-C388-46C1-BF86-8F1CD3C1DE6D}" name="Column1" dataDxfId="8">
+    <tableColumn id="4" xr3:uid="{52D8179B-C388-46C1-BF86-8F1CD3C1DE6D}" name="Column1" dataDxfId="7">
       <calculatedColumnFormula array="1">SUMPRODUCT(Table2[[#This Row],[A]:[B]],_nWeights,--NOT(ISBLANK(Table2[[#This Row],[A]:[B]])))/SUMPRODUCT(--NOT(ISBLANK(Table2[[#This Row],[A]:[B]])),_nWeights)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -724,12 +728,12 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0B41AE75-F469-4876-BA7E-5E7F1983D95B}" name="Table5" displayName="Table5" ref="L47:P56" totalsRowShown="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0B41AE75-F469-4876-BA7E-5E7F1983D95B}" name="Table5" displayName="Table5" ref="L47:P56" totalsRowShown="0" dataDxfId="4">
   <autoFilter ref="L47:P56" xr:uid="{0B41AE75-F469-4876-BA7E-5E7F1983D95B}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{6F1FEBCF-087E-4940-B140-2786436B5C2A}" name="Index" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{43282383-13E8-44B4-BAEC-67D1E60C035F}" name="A" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{EEBF8DC7-6862-4292-90BA-1A7C0873FD79}" name="B" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{6F1FEBCF-087E-4940-B140-2786436B5C2A}" name="Index" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{43282383-13E8-44B4-BAEC-67D1E60C035F}" name="A" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{EEBF8DC7-6862-4292-90BA-1A7C0873FD79}" name="B" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{E0922B13-999D-4174-8C52-DC3493F5F095}" name="C"/>
     <tableColumn id="5" xr3:uid="{FFF68114-22E5-41B7-A342-81EC614187BB}" name="Column" dataDxfId="0">
       <calculatedColumnFormula array="1">Wmean2(Table5[[#This Row],[A]:[C]],_nWeights2)</calculatedColumnFormula>
@@ -927,15 +931,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB114D2F-F620-446A-92CE-0CB3C9FD0F74}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:P56"/>
+  <dimension ref="A1:P60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="S46" sqref="S45:S46"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -946,7 +950,7 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -957,7 +961,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -969,12 +973,12 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -988,7 +992,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1018,7 +1022,7 @@
         <v>=SUMPRODUCT(--NOT(ISBLANK(B8:C8)),$B$7:$C$7,B8:C8)/SUMPRODUCT(--NOT(ISBLANK(B8:C8)),$B$7:$C$7)</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1041,7 +1045,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1064,7 +1068,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1090,7 +1094,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
@@ -1110,7 +1114,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
@@ -1130,7 +1134,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7</v>
       </c>
@@ -1150,7 +1154,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>13</v>
       </c>
@@ -1161,7 +1165,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1172,7 +1176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -1210,7 +1214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1249,7 +1253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2</v>
       </c>
@@ -1289,7 +1293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3</v>
       </c>
@@ -1301,7 +1305,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4</v>
       </c>
@@ -1316,7 +1320,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>5</v>
       </c>
@@ -1325,7 +1329,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6</v>
       </c>
@@ -1334,7 +1338,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>7</v>
       </c>
@@ -1343,12 +1347,12 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -1362,7 +1366,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
@@ -1377,7 +1381,7 @@
         <v>1.3333333333333333</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2</v>
       </c>
@@ -1392,7 +1396,7 @@
         <v>1.3333333333333333</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3</v>
       </c>
@@ -1407,7 +1411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>4</v>
       </c>
@@ -1422,7 +1426,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>5</v>
       </c>
@@ -1437,7 +1441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>6</v>
       </c>
@@ -1452,7 +1456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>7</v>
       </c>
@@ -1467,7 +1471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>14</v>
       </c>
@@ -1475,7 +1479,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="M45" t="s">
         <v>22</v>
       </c>
@@ -1489,7 +1493,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>11</v>
       </c>
@@ -1514,13 +1518,13 @@
       <c r="J47" t="s">
         <v>15</v>
       </c>
-      <c r="L47" s="13" t="s">
+      <c r="L47" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="M47" s="13" t="s">
+      <c r="M47" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="N47" s="13" t="s">
+      <c r="N47" s="11" t="s">
         <v>10</v>
       </c>
       <c r="O47" t="s">
@@ -1530,7 +1534,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1</v>
       </c>
@@ -1557,16 +1561,16 @@
         <f t="array" ref="J48">Wmean(Table245[[#This Row],[A]:[B]])</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="L48" s="12">
-        <v>1</v>
-      </c>
-      <c r="M48" s="12">
-        <v>1</v>
-      </c>
-      <c r="N48" s="12">
-        <v>2</v>
-      </c>
-      <c r="O48" s="8">
+      <c r="L48" s="10">
+        <v>1</v>
+      </c>
+      <c r="M48" s="10">
+        <v>1</v>
+      </c>
+      <c r="N48" s="10">
+        <v>2</v>
+      </c>
+      <c r="O48" s="7">
         <v>1</v>
       </c>
       <c r="P48" cm="1">
@@ -1574,7 +1578,7 @@
         <v>1.0999999999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2</v>
       </c>
@@ -1618,7 +1622,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>3</v>
       </c>
@@ -1659,7 +1663,7 @@
         <v>3.0000000000000004</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>4</v>
       </c>
@@ -1695,7 +1699,7 @@
       <c r="N51" s="5">
         <v>3</v>
       </c>
-      <c r="O51" s="9">
+      <c r="O51" s="8">
         <v>3</v>
       </c>
       <c r="P51" cm="1">
@@ -1703,7 +1707,7 @@
         <v>2.9999999999999996</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>5</v>
       </c>
@@ -1739,7 +1743,7 @@
       <c r="N52" s="4">
         <v>1</v>
       </c>
-      <c r="O52" s="8">
+      <c r="O52" s="7">
         <v>1</v>
       </c>
       <c r="P52" cm="1">
@@ -1747,7 +1751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>6</v>
       </c>
@@ -1783,7 +1787,7 @@
       <c r="N53" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="O53" s="10">
+      <c r="O53">
         <v>2</v>
       </c>
       <c r="P53" cm="1">
@@ -1791,7 +1795,7 @@
         <v>1.2222222222222225</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>7</v>
       </c>
@@ -1827,7 +1831,7 @@
       <c r="N54" s="4">
         <v>1</v>
       </c>
-      <c r="O54" s="8">
+      <c r="O54" s="7">
         <v>1</v>
       </c>
       <c r="P54" cm="1">
@@ -1835,11 +1839,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="G55">
         <v>8</v>
       </c>
-      <c r="J55" s="7" t="e" cm="1">
+      <c r="J55" t="e" cm="1">
         <f t="array" ref="J55">Wmean(Table245[[#This Row],[A]:[B]])</f>
         <v>#DIV/0!</v>
       </c>
@@ -1853,7 +1857,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="G56">
         <v>9</v>
       </c>
@@ -1863,7 +1867,7 @@
       <c r="I56">
         <v>0</v>
       </c>
-      <c r="J56" s="7" t="e" cm="1">
+      <c r="J56" t="e" cm="1">
         <f t="array" ref="J56">Wmean(Table245[[#This Row],[A]:[B]])</f>
         <v>#DIV/0!</v>
       </c>
@@ -1876,12 +1880,22 @@
       <c r="N56" s="4">
         <v>0</v>
       </c>
-      <c r="O56" s="11">
+      <c r="O56" s="9">
         <v>0</v>
       </c>
       <c r="P56" t="e" cm="1">
         <f t="array" ref="P56">Wmean2(Table5[[#This Row],[A]:[C]],_nWeights2)</f>
         <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>